<commit_message>
Admin Inputs through Excel sheet
</commit_message>
<xml_diff>
--- a/Budget Simulation - Admin.xlsx
+++ b/Budget Simulation - Admin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\Budget-Simulation-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD743A2-4DD1-4066-AC49-576938DECFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCBD3EE-2729-475E-871B-6C422DEEE8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4749EA82-5507-43F6-8DEA-C3E93E89C445}"/>
+    <workbookView xWindow="6504" yWindow="936" windowWidth="17280" windowHeight="8880" xr2:uid="{4749EA82-5507-43F6-8DEA-C3E93E89C445}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Simulation - Admin" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -215,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -297,17 +297,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -324,7 +313,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -332,8 +321,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -341,14 +329,11 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -369,6 +354,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -685,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5F08C9-4AC4-4904-88A7-B04373F8F6D6}">
-  <dimension ref="B3:K25"/>
+  <dimension ref="C3:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,139 +692,139 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="3:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="15">
+        <v>30000</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" spans="3:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="C5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E5" s="16">
         <v>0.03</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H5" s="19">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>10</v>
+      </c>
+      <c r="J5" s="10">
+        <v>22000</v>
+      </c>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="3:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="C6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="19">
         <v>2</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C5" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="16">
-        <v>30000</v>
-      </c>
-      <c r="H5" s="21">
-        <v>1</v>
-      </c>
-      <c r="I5" s="10">
-        <v>10</v>
-      </c>
-      <c r="J5" s="11">
-        <v>22000</v>
-      </c>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C6" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="H6" s="21">
-        <v>2</v>
-      </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <v>20</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <f>J5</f>
         <v>22000</v>
       </c>
-      <c r="K6" s="20"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>0.15</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="19">
         <v>3</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>30</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <f>J6</f>
         <v>22000</v>
       </c>
-      <c r="K7" s="24"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>0.02</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="19">
         <v>4</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <v>40</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="14">
         <f>J7</f>
         <v>22000</v>
       </c>
-      <c r="K8" s="24"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>0.06</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="19">
         <v>5</v>
       </c>
       <c r="I9" s="1">
@@ -845,19 +833,19 @@
       <c r="J9" s="2">
         <v>27000</v>
       </c>
-      <c r="K9" s="24"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>0.08</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="19">
         <v>6</v>
       </c>
       <c r="I10" s="3">
@@ -868,13 +856,13 @@
         <f>J9</f>
         <v>27000</v>
       </c>
-      <c r="K10" s="24"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="H11" s="21">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="H11" s="19">
         <v>7</v>
       </c>
       <c r="I11" s="3">
@@ -885,13 +873,13 @@
         <f>J10</f>
         <v>27000</v>
       </c>
-      <c r="K11" s="24"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="H12" s="21">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="H12" s="19">
         <v>8</v>
       </c>
       <c r="I12" s="4">
@@ -902,13 +890,13 @@
         <f>J11</f>
         <v>27000</v>
       </c>
-      <c r="K12" s="24"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="H13" s="21">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="H13" s="19">
         <v>9</v>
       </c>
       <c r="I13" s="3">
@@ -918,13 +906,13 @@
       <c r="J13" s="2">
         <v>20000</v>
       </c>
-      <c r="K13" s="24"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="H14" s="21">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="H14" s="19">
         <v>10</v>
       </c>
       <c r="I14" s="3">
@@ -935,13 +923,13 @@
         <f>J13</f>
         <v>20000</v>
       </c>
-      <c r="K14" s="24"/>
+      <c r="K14" s="22"/>
     </row>
     <row r="15" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="H15" s="21">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="H15" s="19">
         <v>11</v>
       </c>
       <c r="I15" s="3">
@@ -952,13 +940,13 @@
         <f>J14</f>
         <v>20000</v>
       </c>
-      <c r="K15" s="24"/>
+      <c r="K15" s="22"/>
     </row>
     <row r="16" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="H16" s="21">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="H16" s="19">
         <v>12</v>
       </c>
       <c r="I16" s="4">
@@ -969,13 +957,13 @@
         <f>J15</f>
         <v>20000</v>
       </c>
-      <c r="K16" s="25"/>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="H17" s="21">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="H17" s="19">
         <v>13</v>
       </c>
       <c r="I17" s="3">
@@ -985,13 +973,13 @@
       <c r="J17" s="6">
         <v>24000</v>
       </c>
-      <c r="K17" s="24"/>
+      <c r="K17" s="22"/>
     </row>
     <row r="18" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="H18" s="21">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="H18" s="19">
         <v>14</v>
       </c>
       <c r="I18" s="3">
@@ -1002,13 +990,13 @@
         <f>J17</f>
         <v>24000</v>
       </c>
-      <c r="K18" s="24"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="H19" s="21">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="H19" s="19">
         <v>15</v>
       </c>
       <c r="I19" s="3">
@@ -1019,13 +1007,13 @@
         <f>J18</f>
         <v>24000</v>
       </c>
-      <c r="K19" s="24"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="H20" s="21">
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="H20" s="19">
         <v>16</v>
       </c>
       <c r="I20" s="4">
@@ -1036,77 +1024,73 @@
         <f>J19</f>
         <v>24000</v>
       </c>
-      <c r="K20" s="24"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="H21" s="21">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="H21" s="19">
         <v>17</v>
       </c>
       <c r="I21" s="3">
-        <f>I9</f>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J21" s="2">
-        <v>24000</v>
-      </c>
-      <c r="K21" s="24"/>
+        <v>22000</v>
+      </c>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="H22" s="21">
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="H22" s="19">
         <v>18</v>
       </c>
       <c r="I22" s="3">
-        <f>I10</f>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J22" s="2">
         <f>J21</f>
-        <v>24000</v>
-      </c>
-      <c r="K22" s="24"/>
+        <v>22000</v>
+      </c>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" spans="3:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="H23" s="21">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="H23" s="19">
         <v>19</v>
       </c>
       <c r="I23" s="3">
-        <f>I11</f>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J23" s="2">
         <f>J22</f>
-        <v>24000</v>
-      </c>
-      <c r="K23" s="24"/>
+        <v>22000</v>
+      </c>
+      <c r="K23" s="22"/>
     </row>
     <row r="24" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="21">
+      <c r="H24" s="19">
         <v>20</v>
       </c>
-      <c r="I24" s="7">
-        <f>I12</f>
-        <v>67</v>
-      </c>
-      <c r="J24" s="8">
+      <c r="I24" s="3">
+        <v>70</v>
+      </c>
+      <c r="J24" s="7">
         <f>J23</f>
-        <v>24000</v>
-      </c>
-      <c r="K24" s="23"/>
+        <v>22000</v>
+      </c>
+      <c r="K24" s="21"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="H25" s="22"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1119,6 +1103,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1C30AF05D05F44290B877FBA47E06D7" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c390872fb5ee6617233522a93297a75b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cf34c0ae-c264-4763-a50e-62e14a974a4b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7125aa1be032bbebc3f6e2a5c96b98de" ns3:_="">
     <xsd:import namespace="cf34c0ae-c264-4763-a50e-62e14a974a4b"/>
@@ -1250,35 +1249,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24DADEF-2328-413E-AD3E-4515D429BFEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{982C5008-F5A2-4ABF-BFBD-A2038E911280}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cf34c0ae-c264-4763-a50e-62e14a974a4b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1300,9 +1274,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{982C5008-F5A2-4ABF-BFBD-A2038E911280}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F24DADEF-2328-413E-AD3E-4515D429BFEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf34c0ae-c264-4763-a50e-62e14a974a4b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>